<commit_message>
Small tweak for counts.
</commit_message>
<xml_diff>
--- a/docs/EMUFI-Encoding.xlsx
+++ b/docs/EMUFI-Encoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmekonnen/git/emufi/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C446397-314E-EC4E-8D33-B3C437F982AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94889364-C26A-8541-8829-6D9D43ACAE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4400" yWindow="500" windowWidth="32260" windowHeight="23500" activeTab="1" xr2:uid="{9DB3E3F7-9827-3A48-8708-08A04A450073}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="977">
   <si>
     <t>F40X</t>
   </si>
@@ -2961,6 +2961,9 @@
   </si>
   <si>
     <t></t>
+  </si>
+  <si>
+    <t></t>
   </si>
 </sst>
 </file>
@@ -3163,7 +3166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3358,6 +3361,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6825,8 +6831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F02D64-DF73-EA4E-A34C-8BEB5FFED775}">
   <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S70" sqref="S70"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8532,7 +8538,9 @@
       <c r="B32" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="30"/>
+      <c r="C32" s="106" t="s">
+        <v>976</v>
+      </c>
       <c r="D32" s="31"/>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>

</xml_diff>